<commit_message>
added parameters from Excel file
</commit_message>
<xml_diff>
--- a/test3/java_test1.xlsx
+++ b/test3/java_test1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">abc</t>
+    <t xml:space="preserve">https://www.tsx.com</t>
   </si>
   <si>
-    <t xml:space="preserve">def</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ghi</t>
+    <t xml:space="preserve">TMX TSX | TSXV - Toronto Stock Exchange and TSX Venture Exchange</t>
   </si>
 </sst>
 </file>
@@ -43,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,12 +100,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -237,10 +239,13 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="70.68"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -248,14 +253,12 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>